<commit_message>
add more extras: M8 washers, modified endstop holder for limit switches with 24.5mm hole spacing
</commit_message>
<xml_diff>
--- a/printed_parts/output/PrintList.xlsx
+++ b/printed_parts/output/PrintList.xlsx
@@ -78,9 +78,6 @@
     <t>old</t>
   </si>
   <si>
-    <t>1 of 3</t>
-  </si>
-  <si>
     <t>q</t>
   </si>
   <si>
@@ -90,7 +87,10 @@
     <t>mod y tensioner</t>
   </si>
   <si>
-    <t>MISSING</t>
+    <t>q2</t>
+  </si>
+  <si>
+    <t>q2 (X left only)</t>
   </si>
 </sst>
 </file>
@@ -432,7 +432,7 @@
   <dimension ref="B2:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -472,7 +472,7 @@
         <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E5" t="s">
         <v>19</v>
@@ -486,7 +486,7 @@
         <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
@@ -494,7 +494,7 @@
         <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
@@ -502,7 +502,7 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
@@ -510,15 +510,15 @@
         <v>13</v>
       </c>
       <c r="D10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
@@ -529,7 +529,7 @@
         <v>15</v>
       </c>
       <c r="D14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">

</xml_diff>